<commit_message>
Sending mail issue resolved added scrapemail.py
</commit_message>
<xml_diff>
--- a/outputs/1401CB01.xlsx
+++ b/outputs/1401CB01.xlsx
@@ -598,10 +598,10 @@
         </is>
       </c>
       <c r="B11" s="4" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="3" t="n">
         <v>0</v>
@@ -615,15 +615,15 @@
         </is>
       </c>
       <c r="B12" s="4" t="n">
-        <v>84</v>
+        <v>126</v>
       </c>
       <c r="C12" s="5" t="n">
-        <v>-42</v>
+        <v>-28</v>
       </c>
       <c r="D12" s="3" t="inlineStr"/>
       <c r="E12" s="6" t="inlineStr">
         <is>
-          <t>42/168</t>
+          <t>98/252</t>
         </is>
       </c>
     </row>

</xml_diff>